<commit_message>
Add final cob and seed traits for Ames and Crawfordsville
</commit_message>
<xml_diff>
--- a/data/5 Cob Traits Station/Right Station/Inbred/C-2352/5_cob_Traits_04.03.23_MN.xlsx
+++ b/data/5 Cob Traits Station/Right Station/Inbred/C-2352/5_cob_Traits_04.03.23_MN.xlsx
@@ -38,7 +38,7 @@
     <t xml:space="preserve">Station (left or right)</t>
   </si>
   <si>
-    <t xml:space="preserve">cob broke in pieces</t>
+    <t xml:space="preserve">brokenCob</t>
   </si>
   <si>
     <t xml:space="preserve">string used to measure length?</t>
@@ -267,9 +267,9 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>